<commit_message>
Functional Specs and TCRS
</commit_message>
<xml_diff>
--- a/450_SulfurEngine/Documents/TCR.xlsx
+++ b/450_SulfurEngine/Documents/TCR.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sulfur\450_SulfurEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sulfur\450_SulfurEngine\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26250" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="176">
   <si>
     <t>Date</t>
   </si>
@@ -545,9 +545,6 @@
   </si>
   <si>
     <t>A - meets professional expectations</t>
-  </si>
-  <si>
-    <t>Not a tech demo</t>
   </si>
   <si>
     <t>Not a tool development</t>
@@ -921,6 +918,15 @@
   </si>
   <si>
     <t>Dylan Norris, Maxim Kolesnik</t>
+  </si>
+  <si>
+    <t>Tech demo</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Not a game project</t>
   </si>
 </sst>
 </file>
@@ -1751,6 +1757,42 @@
     <xf numFmtId="164" fontId="1" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1772,41 +1814,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1819,9 +1828,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2523,7 +2529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2541,73 +2547,73 @@
   <sheetData>
     <row r="1" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="25"/>
-      <c r="B1" s="90" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="B1" s="102" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
     </row>
     <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="91" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="103" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="93" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
+      <c r="B3" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
     </row>
     <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="93" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
+      <c r="B4" s="105" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="111" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
+      <c r="B5" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="88" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
+      <c r="B6" s="100" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="95"/>
+      <c r="B8" s="96"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
@@ -2618,10 +2624,10 @@
       <c r="C9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="98"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
@@ -2632,24 +2638,24 @@
       <c r="C10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="99" t="s">
+      <c r="D10" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="100"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="42">
         <f>TCRs!F4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="100"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
@@ -2660,10 +2666,10 @@
       <c r="C12" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="102"/>
+      <c r="E12" s="95"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
@@ -2674,10 +2680,10 @@
       <c r="C13" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="99" t="s">
+      <c r="D13" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="100"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36"/>
@@ -2688,16 +2694,16 @@
       <c r="C14" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="104"/>
+      <c r="E14" s="99"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="96"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2706,15 +2712,15 @@
       <c r="A16" s="36"/>
       <c r="B16" s="37">
         <f>DCRs!F2</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="D16" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="98"/>
+      <c r="E16" s="91"/>
     </row>
     <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
@@ -2725,10 +2731,10 @@
       <c r="C17" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="100"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
@@ -2739,10 +2745,10 @@
       <c r="C18" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="99" t="s">
+      <c r="D18" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="100"/>
+      <c r="E18" s="93"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
@@ -2753,24 +2759,24 @@
       <c r="C19" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="100"/>
+      <c r="E19" s="93"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="43">
         <f>DCRs!F6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="101" t="s">
+      <c r="D20" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="102"/>
+      <c r="E20" s="95"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
@@ -2781,34 +2787,33 @@
       <c r="C21" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="99" t="s">
+      <c r="D21" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="100"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
       <c r="B22" s="39">
         <f>DCRs!F8</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="105" t="s">
+      <c r="D22" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="106"/>
+      <c r="E22" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="D9:E9"/>
@@ -2817,12 +2822,13 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:C11 C13:C14">
     <cfRule type="cellIs" dxfId="51" priority="22" operator="equal">
@@ -2889,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,7 +2984,7 @@
       <c r="E4" s="56"/>
       <c r="F4" s="17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>75</v>
@@ -2999,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" s="63">
         <f t="shared" si="1"/>
@@ -3080,7 +3086,7 @@
         <v>86</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" s="78" t="s">
         <v>138</v>
@@ -3101,7 +3107,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="15" t="s">
@@ -3124,7 +3130,7 @@
         <v>99</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>74</v>
@@ -3143,10 +3149,10 @@
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>138</v>
@@ -3175,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3191,7 +3197,7 @@
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>5</v>
@@ -3355,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3405,7 +3411,7 @@
       <c r="E2" s="59"/>
       <c r="F2" s="62">
         <f>COUNTIF($F$10:$F$25,$G2)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>129</v>
@@ -3474,10 +3480,10 @@
       <c r="E6" s="55"/>
       <c r="F6" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H6" s="63">
         <f t="shared" si="1"/>
@@ -3510,7 +3516,7 @@
       <c r="E8" s="58"/>
       <c r="F8" s="84">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" s="76" t="s">
         <v>74</v>
@@ -3542,10 +3548,10 @@
       <c r="G9" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="108" t="s">
+      <c r="H9" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="109"/>
+      <c r="I9" s="110"/>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="85" t="s">
@@ -3567,8 +3573,8 @@
       <c r="G10" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -3581,17 +3587,17 @@
         <v>102</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="15" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="G11" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="108"/>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
@@ -3604,17 +3610,17 @@
         <v>102</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="15" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="G12" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="108"/>
     </row>
     <row r="13" spans="1:9" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -3627,17 +3633,19 @@
         <v>102</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="22"/>
+        <v>146</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>173</v>
+      </c>
       <c r="F13" s="15" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="108"/>
     </row>
     <row r="14" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -3652,17 +3660,15 @@
       <c r="D14" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>139</v>
-      </c>
+      <c r="E14"/>
       <c r="F14" s="15" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="G14" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
@@ -3677,17 +3683,15 @@
       <c r="D15" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="29" t="s">
-        <v>139</v>
-      </c>
+      <c r="E15"/>
       <c r="F15" s="15" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="G15" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -3702,17 +3706,17 @@
       <c r="D16" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>139</v>
+      <c r="E16" t="s">
+        <v>174</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="G16" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
@@ -3728,7 +3732,7 @@
         <v>114</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>74</v>
@@ -3736,8 +3740,8 @@
       <c r="G17" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
@@ -3753,7 +3757,7 @@
         <v>115</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>74</v>
@@ -3761,8 +3765,8 @@
       <c r="G18" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
@@ -3778,7 +3782,7 @@
         <v>116</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>74</v>
@@ -3786,8 +3790,8 @@
       <c r="G19" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="107"/>
-      <c r="I19" s="107"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
     </row>
     <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
@@ -3803,7 +3807,7 @@
         <v>123</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>74</v>
@@ -3811,8 +3815,8 @@
       <c r="G20" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
     </row>
     <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -3828,7 +3832,7 @@
         <v>124</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>74</v>
@@ -3836,8 +3840,8 @@
       <c r="G21" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
     </row>
     <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
@@ -3853,7 +3857,7 @@
         <v>125</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>74</v>
@@ -3861,8 +3865,8 @@
       <c r="G22" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="107"/>
-      <c r="I22" s="107"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="108"/>
     </row>
     <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3877,15 +3881,17 @@
       <c r="D23" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="22" t="s">
+        <v>175</v>
+      </c>
       <c r="F23" s="15" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="G23" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="108"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3900,15 +3906,17 @@
       <c r="D24" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="22" t="s">
+        <v>175</v>
+      </c>
       <c r="F24" s="15" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="G24" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="108"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
@@ -3923,15 +3931,17 @@
       <c r="D25" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="22"/>
+      <c r="E25" s="22" t="s">
+        <v>175</v>
+      </c>
       <c r="F25" s="15" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="G25" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="H25" s="107"/>
-      <c r="I25" s="107"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="108"/>
     </row>
     <row r="26" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
@@ -3947,7 +3957,7 @@
         <v>123</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>74</v>
@@ -3955,8 +3965,8 @@
       <c r="G26" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="108"/>
     </row>
     <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -3972,7 +3982,7 @@
         <v>125</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>74</v>
@@ -3980,8 +3990,8 @@
       <c r="G27" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
     </row>
     <row r="28" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -3997,7 +4007,7 @@
         <v>128</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>74</v>
@@ -4005,19 +4015,11 @@
       <c r="G28" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H27:I27"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
@@ -4030,6 +4032,14 @@
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <conditionalFormatting sqref="F29:G1048576 F1:G9">
     <cfRule type="cellIs" dxfId="31" priority="57" operator="equal">
@@ -4162,8 +4172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4365,7 +4375,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>67</v>
@@ -4373,7 +4383,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>16</v>
@@ -4386,10 +4396,10 @@
       </c>
       <c r="E2" s="49"/>
       <c r="F2" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="49" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>151</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -4406,7 +4416,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>21</v>
@@ -4429,13 +4439,13 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>23</v>
@@ -4452,7 +4462,7 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>25</v>
@@ -4475,13 +4485,13 @@
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="18" t="s">
@@ -4507,13 +4517,13 @@
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>30</v>
@@ -4530,13 +4540,13 @@
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>30</v>
@@ -4553,7 +4563,7 @@
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>33</v>
@@ -4576,7 +4586,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>35</v>
@@ -4610,7 +4620,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>40</v>
@@ -4627,7 +4637,7 @@
     </row>
     <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>41</v>
@@ -4648,7 +4658,7 @@
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>42</v>
@@ -4680,13 +4690,13 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>37</v>
@@ -4726,13 +4736,13 @@
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>47</v>
@@ -4760,7 +4770,7 @@
     </row>
     <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>49</v>
@@ -4783,17 +4793,17 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the last tcr update
</commit_message>
<xml_diff>
--- a/450_SulfurEngine/Documents/TCR.xlsx
+++ b/450_SulfurEngine/Documents/TCR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26250" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26250" windowHeight="11025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1751,6 +1751,42 @@
     <xf numFmtId="164" fontId="1" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1774,42 +1810,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2523,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2541,67 +2541,67 @@
   <sheetData>
     <row r="1" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="25"/>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
     </row>
     <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="103" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="92"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
     </row>
     <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="105" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
     </row>
     <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="106"/>
     </row>
     <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="96" t="s">
@@ -2618,10 +2618,10 @@
       <c r="C9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="99"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
@@ -2632,10 +2632,10 @@
       <c r="C10" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="100" t="s">
+      <c r="D10" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="101"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
@@ -2646,10 +2646,10 @@
       <c r="C11" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="101"/>
+      <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
@@ -2660,10 +2660,10 @@
       <c r="C12" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="103"/>
+      <c r="E12" s="95"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
@@ -2674,10 +2674,10 @@
       <c r="C13" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="101"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36"/>
@@ -2688,10 +2688,10 @@
       <c r="C14" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="105"/>
+      <c r="E14" s="99"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="97" t="s">
@@ -2711,10 +2711,10 @@
       <c r="C16" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="99"/>
+      <c r="E16" s="91"/>
     </row>
     <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
@@ -2725,10 +2725,10 @@
       <c r="C17" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="101"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
@@ -2739,10 +2739,10 @@
       <c r="C18" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D18" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="101"/>
+      <c r="E18" s="93"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
@@ -2753,10 +2753,10 @@
       <c r="C19" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="101"/>
+      <c r="E19" s="93"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
@@ -2767,10 +2767,10 @@
       <c r="C20" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="103"/>
+      <c r="E20" s="95"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
@@ -2781,10 +2781,10 @@
       <c r="C21" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D21" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="101"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
@@ -2795,20 +2795,19 @@
       <c r="C22" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="106" t="s">
+      <c r="D22" s="88" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="107"/>
+      <c r="E22" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="D9:E9"/>
@@ -2817,12 +2816,13 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:C11 C13:C14">
     <cfRule type="cellIs" dxfId="51" priority="22" operator="equal">
@@ -4014,14 +4014,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H27:I27"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
@@ -4034,6 +4026,14 @@
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <conditionalFormatting sqref="F29:G1048576 F1:G9">
     <cfRule type="cellIs" dxfId="31" priority="57" operator="equal">
@@ -4166,8 +4166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>29</v>

</xml_diff>